<commit_message>
Early childhood education text changes.
</commit_message>
<xml_diff>
--- a/dashboard_loader/education_uaece_uploader/education_uaece.xlsx
+++ b/dashboard_loader/education_uaece_uploader/education_uaece.xlsx
@@ -112,31 +112,48 @@
   <si>
     <r>
       <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
+        <sz val="12"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="1"/>
       </rPr>
-      <t xml:space="preserve">Preschool enrolment rates reported in the </t>
+      <t xml:space="preserve">Preschool enrolment rates reported </t>
     </r>
     <r>
       <rPr>
-        <i val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="1"/>
       </rPr>
-      <t xml:space="preserve">Report on Government Services </t>
+      <t xml:space="preserve">under the NIRA </t>
     </r>
     <r>
       <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
+        <sz val="12"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="1"/>
       </rPr>
-      <t xml:space="preserve">2018 vary from the National Partnership results. The (newer) methodology used in RoGS 2018 incorporates state-specific Year Before Full-Time School cut-off dates, which affect the number of children counted. The National Partnership has kept the existing enrolment rate methodology to maintain reporting consistency across the term of several successive agreements.    </t>
+      <t xml:space="preserve">and in the Report on Government Services 2018 vary from the National Partnership results. The (newer) methodology used in RoGS </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">and the NIRA </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">incorporates state-specific Year Before Full-Time School cut-off dates, which affect the number of children counted. The National Partnership has kept the existing enrolment rate methodology to maintain reporting consistency across the term of several successive agreements.</t>
     </r>
   </si>
   <si>
@@ -162,7 +179,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -198,11 +215,16 @@
       <charset val="1"/>
     </font>
     <font>
-      <i val="true"/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
+      <sz val="12"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -258,7 +280,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -271,10 +293,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -291,12 +309,12 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -309,6 +327,66 @@
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
     <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0070C0"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -476,34 +554,34 @@
       <c r="B6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="3" t="n">
-        <v>100</v>
-      </c>
-      <c r="D6" s="3" t="n">
-        <v>100</v>
-      </c>
-      <c r="E6" s="3" t="n">
-        <v>100</v>
-      </c>
-      <c r="F6" s="3" t="n">
-        <v>100</v>
-      </c>
-      <c r="G6" s="3" t="n">
-        <v>100</v>
-      </c>
-      <c r="H6" s="3" t="n">
-        <v>100</v>
-      </c>
-      <c r="I6" s="3" t="n">
-        <v>100</v>
-      </c>
-      <c r="J6" s="3" t="n">
+      <c r="C6" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="E6" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="F6" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="G6" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="H6" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="I6" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="J6" s="2" t="n">
         <v>100</v>
       </c>
       <c r="K6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="n">
+      <c r="A7" s="3" t="n">
         <v>2016</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -554,104 +632,104 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="5" width="10.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="5" width="91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="5" width="9.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="10.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="4" width="9.11"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="7" t="n">
+      <c r="B4" s="6" t="n">
         <v>2016</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="40.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="66.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="s">
+    <row r="6" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="40.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="6" t="s">
+    <row r="7" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="40.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="8" t="s">
+    <row r="8" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="53.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="8" t="s">
+    <row r="9" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="66.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="8" t="s">
+    <row r="10" customFormat="false" ht="72.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="7" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5" t="s">
+    <row r="11" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="9" t="s">
+    <row r="12" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="8" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="9" t="s">
+    <row r="13" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="8" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="9" t="s">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="8" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Dat updates to uaece and legal assistance.
</commit_message>
<xml_diff>
--- a/dashboard_loader/education_uaece_uploader/education_uaece.xlsx
+++ b/dashboard_loader/education_uaece_uploader/education_uaece.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
   <si>
     <t xml:space="preserve">Increase the proportion of children enrolled in the year before full-time school in quality early childhood education programme(s) to 95%</t>
   </si>
@@ -77,7 +77,7 @@
     <t xml:space="preserve">Short title</t>
   </si>
   <si>
-    <t xml:space="preserve">Provide universal access to preschool.</t>
+    <t xml:space="preserve">Provide universal access to preschool</t>
   </si>
   <si>
     <t xml:space="preserve">Status</t>
@@ -92,7 +92,34 @@
     <t xml:space="preserve">Desc Body</t>
   </si>
   <si>
-    <t xml:space="preserve">Since 2008, substantial progress has been made towards achieving universal access to preschool programs for Australian children in the year before full-time school. In 2016, all jurisdictions exceeded the 95 per cent benchmark and achieved either full, or close to full, enrolment.</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Since 2008, substantial progress has been made towards achieving universal access to preschool programs for Australian children in the year before full-time school. In </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2017,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> all jurisdictions exceeded the 95 per cent benchmark and achieved either full, or close to full, enrolment.</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Notes</t>
@@ -112,58 +139,157 @@
   <si>
     <r>
       <rPr>
-        <sz val="12"/>
-        <color rgb="FF0070C0"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Preschool enrolment rates reported </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">under the NIRA</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">and</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> in the </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Report on Government Services </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2018 vary from the National Partnership results. The (newer) methodology used in RoGS </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">and the NIRA</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> incorporates state-specific Year Before Full-Time School cut-off dates, which affect the number of children counted. The National Partnership has kept the existing enrolment rate methodology to maintain reporting consistency across the term of several successive agreements.    </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Source</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2008 data from National Partnership Agreement on Early Childhood Education State and Territory Bilateral Agreements. </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">Preschool enrolment rates reported </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2015</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">under the NIRA </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF0070C0"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">and in the Report on Government Services 2018 vary from the National Partnership results. The (newer) methodology used in RoGS </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> 2016 and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">and the NIRA </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF0070C0"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2017</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">incorporates state-specific Year Before Full-Time School cut-off dates, which affect the number of children counted. The National Partnership has kept the existing enrolment rate methodology to maintain reporting consistency across the term of several successive agreements.</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Source</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2008 data from National Partnership Agreement on Early Childhood Education State and Territory Bilateral Agreements. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2015 and 2016  data from the National Early Childhood Education and Care Collection (ABS Cat. no. 4240.0) and ABS Estimated Residential Population (ABS Cat. no. 1367.0 and ABS Cat. no. 3101.0)</t>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">  data from the National Early Childhood Education and Care Collection (ABS Cat. no. 4240.0) and ABS Estimated Residential Population (ABS Cat. no. 1367.0 and ABS Cat. no. 3101.0)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">.</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">ABS Estimates and Projections, Aboriginal and Torres Strait Islander Australians, 2001 to 2026 (ABS Cat. no. 3238.0) and ABS Population by Age and Sex, Regions of Australia (ABS Cat. no. 3235.0). </t>
@@ -179,7 +305,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -204,6 +330,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -215,16 +348,18 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF0070C0"/>
-      <name val="Calibri"/>
-      <family val="1"/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="1"/>
+      <i val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -280,7 +415,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -293,28 +428,40 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -327,66 +474,6 @@
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
     <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
-      <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0070C0"/>
-      <rgbColor rgb="FFCCCCFF"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
-      <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
-      <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -395,10 +482,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -554,64 +641,97 @@
       <c r="B6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="2" t="n">
-        <v>100</v>
-      </c>
-      <c r="D6" s="2" t="n">
-        <v>100</v>
-      </c>
-      <c r="E6" s="2" t="n">
-        <v>100</v>
-      </c>
-      <c r="F6" s="2" t="n">
-        <v>100</v>
-      </c>
-      <c r="G6" s="2" t="n">
-        <v>100</v>
-      </c>
-      <c r="H6" s="2" t="n">
-        <v>100</v>
-      </c>
-      <c r="I6" s="2" t="n">
-        <v>100</v>
-      </c>
-      <c r="J6" s="2" t="n">
+      <c r="C6" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="D6" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="E6" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="F6" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="G6" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="H6" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="I6" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="J6" s="3" t="n">
         <v>100</v>
       </c>
       <c r="K6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="n">
+      <c r="A7" s="2" t="n">
+        <v>2017</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="4" t="n">
+        <v>100</v>
+      </c>
+      <c r="D7" s="4" t="n">
+        <v>99</v>
+      </c>
+      <c r="E7" s="4" t="n">
+        <v>100</v>
+      </c>
+      <c r="F7" s="4" t="n">
+        <v>100</v>
+      </c>
+      <c r="G7" s="4" t="n">
+        <v>100</v>
+      </c>
+      <c r="H7" s="4" t="n">
+        <v>100</v>
+      </c>
+      <c r="I7" s="4" t="n">
+        <v>100</v>
+      </c>
+      <c r="J7" s="4" t="n">
+        <v>100</v>
+      </c>
+      <c r="K7" s="2"/>
+    </row>
+    <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="5" t="n">
         <v>2016</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="2" t="n">
+      <c r="C8" s="2" t="n">
         <v>95</v>
       </c>
-      <c r="D7" s="2" t="n">
+      <c r="D8" s="2" t="n">
         <v>95</v>
       </c>
-      <c r="E7" s="2" t="n">
+      <c r="E8" s="2" t="n">
         <v>95</v>
       </c>
-      <c r="F7" s="2" t="n">
+      <c r="F8" s="2" t="n">
         <v>95</v>
       </c>
-      <c r="G7" s="2" t="n">
+      <c r="G8" s="2" t="n">
         <v>95</v>
       </c>
-      <c r="H7" s="2" t="n">
+      <c r="H8" s="2" t="n">
         <v>95</v>
       </c>
-      <c r="I7" s="2" t="n">
+      <c r="I8" s="2" t="n">
         <v>95</v>
       </c>
-      <c r="J7" s="2" t="n">
+      <c r="J8" s="2" t="n">
         <v>95</v>
       </c>
-      <c r="K7" s="2"/>
+      <c r="K8" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -631,105 +751,105 @@
   </sheetPr>
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="10.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="4" width="9.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="10.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="6" width="91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="6" width="9.11"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="7" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="7" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="7" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="6" t="n">
-        <v>2016</v>
+      <c r="B4" s="8" t="n">
+        <v>2017</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="40.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="9" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
+    <row r="6" customFormat="false" ht="66.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="5" t="s">
+    <row r="7" customFormat="false" ht="40.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="5" t="s">
+    <row r="8" customFormat="false" ht="40.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="9" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="5" t="s">
+    <row r="9" customFormat="false" ht="53.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="9" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="72.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="7" t="s">
+    <row r="10" customFormat="false" ht="66.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="9" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4" t="s">
+    <row r="11" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="10" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="8" t="s">
+    <row r="12" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="10" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="8" t="s">
+    <row r="13" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="10" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="8" t="s">
+    <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="11" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Education UAECE minor correction.
</commit_message>
<xml_diff>
--- a/dashboard_loader/education_uaece_uploader/education_uaece.xlsx
+++ b/dashboard_loader/education_uaece_uploader/education_uaece.xlsx
@@ -330,13 +330,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -485,7 +485,7 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+      <selection pane="topLeft" activeCell="G21" activeCellId="0" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -677,12 +677,12 @@
       <c r="C7" s="4" t="n">
         <v>100</v>
       </c>
-      <c r="D7" s="4" t="n">
+      <c r="D7" s="5" t="n">
+        <v>100</v>
+      </c>
+      <c r="E7" s="5" t="n">
         <v>99</v>
       </c>
-      <c r="E7" s="4" t="n">
-        <v>100</v>
-      </c>
       <c r="F7" s="4" t="n">
         <v>100</v>
       </c>
@@ -701,7 +701,7 @@
       <c r="K7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="n">
+      <c r="A8" s="4" t="n">
         <v>2016</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -751,7 +751,7 @@
   </sheetPr>
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>

</xml_diff>